<commit_message>
#1 all code class changes are commited
</commit_message>
<xml_diff>
--- a/training-plan/training-plan.xlsx
+++ b/training-plan/training-plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\personal\Trainings\training-plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B640DA0-282C-4745-8783-692CE003CB80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896F1A00-7FCB-41DF-ABBB-3881C1B26A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92368214-7B83-43B0-AFD6-7A0AFAF29B80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="171">
   <si>
     <t>S no</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>To learn about the diff between a stand alone app and a web app</t>
-  </si>
-  <si>
-    <t>Karun Karthik</t>
   </si>
   <si>
     <t>Completed</t>
@@ -643,10 +640,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554340DC-D259-413E-90A8-D97F337BD015}">
   <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,19 +1011,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>30</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1034,117 +1031,117 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>30</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>40</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>30</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7">
         <v>60</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8">
         <v>60</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>12</v>
+      <c r="G8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1152,231 +1149,231 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>10</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>20</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>10</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>15</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>5</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>10</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>10</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18">
         <v>15</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>20</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20">
         <v>30</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>31</v>
+      <c r="G20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1384,278 +1381,278 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
       <c r="F21">
         <v>15</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23">
         <v>10</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24">
         <v>10</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25">
         <v>10</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26">
         <v>10</v>
       </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27">
         <v>10</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28">
         <v>10</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29">
         <v>15</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30">
         <v>10</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>44</v>
-      </c>
       <c r="F31">
         <v>10</v>
       </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s">
-        <v>46</v>
-      </c>
       <c r="F32">
         <v>15</v>
       </c>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>166</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>15</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34">
-        <v>15</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>49</v>
+      <c r="H34" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -1663,214 +1660,214 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35">
         <v>20</v>
       </c>
       <c r="G35" s="5"/>
-      <c r="H35" s="8"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36">
         <v>15</v>
       </c>
       <c r="G36" s="5"/>
-      <c r="H36" s="8"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37">
         <v>10</v>
       </c>
       <c r="G37" s="5"/>
-      <c r="H37" s="8"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s">
-        <v>54</v>
-      </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F38">
         <v>15</v>
       </c>
       <c r="G38" s="5"/>
-      <c r="H38" s="8"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39">
         <v>20</v>
       </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="8"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40">
         <v>15</v>
       </c>
       <c r="G40" s="5"/>
-      <c r="H40" s="8"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F41">
         <v>15</v>
       </c>
       <c r="G41" s="5"/>
-      <c r="H41" s="8"/>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42">
         <v>15</v>
       </c>
       <c r="G42" s="5"/>
-      <c r="H42" s="8"/>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
         <v>10</v>
       </c>
       <c r="G43" s="5"/>
-      <c r="H43" s="8"/>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>10</v>
       </c>
       <c r="G44" s="5"/>
-      <c r="H44" s="8"/>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45">
         <v>20</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="8">
         <v>44260</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="8">
         <v>44260</v>
       </c>
     </row>
@@ -1879,176 +1876,176 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46">
         <v>10</v>
       </c>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47">
         <v>10</v>
       </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48">
         <v>15</v>
       </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49">
         <v>10</v>
       </c>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50">
         <v>15</v>
       </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
     </row>
     <row r="51" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51">
         <v>10</v>
       </c>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52">
         <v>10</v>
       </c>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53">
         <v>10</v>
       </c>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
         <v>74</v>
       </c>
-      <c r="C54" t="s">
-        <v>167</v>
-      </c>
-      <c r="D54" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" t="s">
-        <v>75</v>
-      </c>
       <c r="F54">
         <v>15</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="8">
         <v>44321</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54" s="8">
         <v>44321</v>
       </c>
     </row>
@@ -2057,544 +2054,544 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55">
         <v>10</v>
       </c>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56">
         <v>10</v>
       </c>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57">
         <v>15</v>
       </c>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58">
         <v>15</v>
       </c>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59">
         <v>10</v>
       </c>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
     </row>
     <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60">
         <v>15</v>
       </c>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F61">
         <v>20</v>
       </c>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62">
         <v>10</v>
       </c>
-      <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63">
         <v>15</v>
       </c>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64">
         <v>10</v>
       </c>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65">
         <v>10</v>
       </c>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66">
         <v>10</v>
       </c>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
     </row>
     <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67">
         <v>15</v>
       </c>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68">
         <v>15</v>
       </c>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69">
         <v>10</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="8">
         <v>44382</v>
       </c>
-      <c r="H69" s="9"/>
+      <c r="H69" s="8"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C70" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F70">
         <v>15</v>
       </c>
-      <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F71">
         <v>15</v>
       </c>
-      <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72">
         <v>20</v>
       </c>
-      <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F73">
         <v>15</v>
       </c>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D74" t="s">
-        <v>10</v>
-      </c>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F75">
         <v>15</v>
       </c>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>77</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F76">
         <v>15</v>
       </c>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>78</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F77">
         <v>15</v>
       </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>74</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F78">
         <v>15</v>
       </c>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>75</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79">
         <v>15</v>
       </c>
-      <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>76</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80">
         <v>15</v>
       </c>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F81">
         <v>15</v>
       </c>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F82">
         <v>15</v>
       </c>
-      <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
     </row>
     <row r="83" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F83" s="5">
         <v>15</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H83" s="7"/>
     </row>
@@ -2603,13 +2600,13 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" s="5">
         <v>15</v>
@@ -2622,13 +2619,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F85" s="5">
         <v>15</v>
@@ -2641,13 +2638,13 @@
         <v>83</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F86" s="5">
         <v>15</v>
@@ -2660,13 +2657,13 @@
         <v>84</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F87" s="5">
         <v>15</v>
@@ -2679,13 +2676,13 @@
         <v>85</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C88" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F88" s="5">
         <v>15</v>
@@ -2698,13 +2695,13 @@
         <v>86</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F89">
         <v>15</v>
@@ -2715,13 +2712,13 @@
         <v>87</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F90">
         <v>15</v>
@@ -2732,13 +2729,13 @@
         <v>88</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C91" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F91">
         <v>15</v>
@@ -2749,13 +2746,13 @@
         <v>89</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F92">
         <v>15</v>
@@ -2766,13 +2763,13 @@
         <v>90</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F93">
         <v>15</v>
@@ -2783,13 +2780,13 @@
         <v>91</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D94" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F94">
         <v>15</v>
@@ -2803,13 +2800,13 @@
         <v>92</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C95" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D95" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F95">
         <v>15</v>
@@ -2820,13 +2817,13 @@
         <v>93</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C96" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D96" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F96">
         <v>15</v>
@@ -2837,13 +2834,13 @@
         <v>94</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C97" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D97" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F97">
         <v>15</v>
@@ -2854,13 +2851,13 @@
         <v>95</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C98" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F98">
         <v>15</v>
@@ -2871,13 +2868,13 @@
         <v>96</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C99" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F99">
         <v>15</v>
@@ -2888,13 +2885,13 @@
         <v>97</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C100" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D100" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F100">
         <v>15</v>
@@ -2908,13 +2905,13 @@
         <v>98</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C101" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D101" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F101">
         <v>15</v>
@@ -2925,13 +2922,13 @@
         <v>99</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C102" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D102" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F102">
         <v>15</v>
@@ -2942,13 +2939,13 @@
         <v>100</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C103" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D103" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F103">
         <v>15</v>
@@ -2959,13 +2956,13 @@
         <v>101</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C104" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F104">
         <v>15</v>
@@ -2976,13 +2973,13 @@
         <v>102</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C105" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F105">
         <v>15</v>
@@ -2993,13 +2990,13 @@
         <v>103</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F106">
         <v>15</v>
@@ -3013,13 +3010,13 @@
         <v>104</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C107" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D107" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F107">
         <v>15</v>
@@ -3030,13 +3027,13 @@
         <v>105</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C108" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D108" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F108">
         <v>15</v>
@@ -3047,13 +3044,13 @@
         <v>106</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F109">
         <v>15</v>
@@ -3064,13 +3061,13 @@
         <v>107</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C110" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F110">
         <v>15</v>
@@ -3081,13 +3078,13 @@
         <v>108</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F111">
         <v>15</v>
@@ -3098,13 +3095,13 @@
         <v>109</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C112" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D112" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F112">
         <v>15</v>
@@ -3118,13 +3115,13 @@
         <v>110</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C113" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F113">
         <v>15</v>
@@ -3135,13 +3132,13 @@
         <v>111</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C114" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F114">
         <v>15</v>
@@ -3152,13 +3149,13 @@
         <v>112</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C115" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D115" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F115">
         <v>120</v>
@@ -3169,13 +3166,13 @@
         <v>113</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F116" s="5">
         <v>180</v>
@@ -3186,7 +3183,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -3194,13 +3191,13 @@
         <v>114</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C118" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D118" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F118">
         <v>15</v>
@@ -3214,13 +3211,13 @@
         <v>115</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C119" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D119" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F119">
         <v>10</v>
@@ -3231,13 +3228,13 @@
         <v>116</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C120" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D120" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F120">
         <v>10</v>
@@ -3248,13 +3245,13 @@
         <v>117</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C121" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D121" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F121">
         <v>15</v>
@@ -3265,13 +3262,13 @@
         <v>118</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C122" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F122">
         <v>15</v>
@@ -3282,13 +3279,13 @@
         <v>119</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C123" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D123" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F123">
         <v>15</v>
@@ -3299,13 +3296,13 @@
         <v>120</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C124" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D124" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F124">
         <v>15</v>
@@ -3316,13 +3313,13 @@
         <v>121</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C125" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D125" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F125">
         <v>15</v>
@@ -3336,13 +3333,13 @@
         <v>122</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C126" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D126" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F126">
         <v>15</v>
@@ -3353,13 +3350,13 @@
         <v>123</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C127" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F127">
         <v>15</v>
@@ -3370,13 +3367,13 @@
         <v>124</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C128" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D128" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F128">
         <v>15</v>
@@ -3387,13 +3384,13 @@
         <v>125</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C129" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D129" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F129">
         <v>15</v>
@@ -3404,13 +3401,13 @@
         <v>126</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C130" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D130" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F130">
         <v>15</v>
@@ -3421,13 +3418,13 @@
         <v>127</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C131" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D131" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F131">
         <v>15</v>
@@ -3441,13 +3438,13 @@
         <v>128</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C132" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D132" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F132">
         <v>15</v>
@@ -3458,13 +3455,13 @@
         <v>129</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C133" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D133" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F133">
         <v>15</v>
@@ -3475,13 +3472,13 @@
         <v>130</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C134" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D134" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F134">
         <v>15</v>
@@ -3492,13 +3489,13 @@
         <v>131</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C135" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D135" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F135">
         <v>15</v>
@@ -3509,13 +3506,13 @@
         <v>132</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C136" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D136" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F136">
         <v>15</v>
@@ -3526,13 +3523,13 @@
         <v>133</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C137" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D137" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F137">
         <v>15</v>
@@ -3543,13 +3540,13 @@
         <v>134</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C138" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D138" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F138">
         <v>15</v>
@@ -3557,7 +3554,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -3565,13 +3562,13 @@
         <v>135</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C140" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D140" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F140">
         <v>30</v>
@@ -3585,13 +3582,13 @@
         <v>136</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C141" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D141" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F141">
         <v>15</v>
@@ -3602,13 +3599,13 @@
         <v>137</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C142" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D142" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F142">
         <v>15</v>
@@ -3619,13 +3616,13 @@
         <v>138</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C143" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D143" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F143">
         <v>10</v>
@@ -3636,13 +3633,13 @@
         <v>139</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C144" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D144" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F144">
         <v>10</v>
@@ -3653,13 +3650,13 @@
         <v>140</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D145" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F145">
         <v>10</v>
@@ -3670,13 +3667,13 @@
         <v>141</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C146" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D146" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F146">
         <v>30</v>
@@ -3690,13 +3687,13 @@
         <v>142</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C147" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D147" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F147">
         <v>10</v>
@@ -3707,13 +3704,13 @@
         <v>143</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C148" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D148" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F148">
         <v>10</v>
@@ -3724,13 +3721,13 @@
         <v>144</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C149" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D149" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F149">
         <v>20</v>
@@ -3741,13 +3738,13 @@
         <v>145</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C150" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D150" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F150">
         <v>20</v>
@@ -3758,13 +3755,13 @@
         <v>146</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C151" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D151" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F151">
         <v>10</v>
@@ -3775,13 +3772,13 @@
         <v>147</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C152" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D152" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F152">
         <v>30</v>
@@ -3789,6 +3786,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="G8:G19"/>
+    <mergeCell ref="H8:H19"/>
+    <mergeCell ref="G20:G33"/>
+    <mergeCell ref="H20:H33"/>
     <mergeCell ref="G69:G82"/>
     <mergeCell ref="H69:H82"/>
     <mergeCell ref="H34:H44"/>
@@ -3796,12 +3799,6 @@
     <mergeCell ref="H45:H53"/>
     <mergeCell ref="G54:G68"/>
     <mergeCell ref="H54:H68"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="G8:G19"/>
-    <mergeCell ref="H8:H19"/>
-    <mergeCell ref="G20:G33"/>
-    <mergeCell ref="H20:H33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>